<commit_message>
Added Visible State support
VisibleState is now a property on IExcelDataReader as well as the Xls
and Xlsx document classes.
VisibleState can be accessed from a DataTable produced by AsDataSet() by
using extended property "visiblestate".
</commit_message>
<xml_diff>
--- a/Excel.Tests.4.5/Resources/Test_Excel_Dataset.xlsx
+++ b/Excel.Tests.4.5/Resources/Test_Excel_Dataset.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="test.csv" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="veryHidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>column a</t>
   </si>
@@ -38,12 +38,15 @@
   <si>
     <t xml:space="preserve"> e </t>
   </si>
+  <si>
+    <t>somedata</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -81,6 +84,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -431,14 +439,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
@@ -447,7 +456,7 @@
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -484,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -504,7 +513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -524,7 +533,7 @@
         <v>41196</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -549,7 +558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -574,7 +583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -599,7 +608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -624,7 +633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -649,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -674,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -699,7 +708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -724,7 +733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -749,7 +758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -774,7 +783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -799,7 +808,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -824,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -849,7 +858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -874,7 +883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -899,7 +908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -924,7 +933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -949,7 +958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -974,7 +983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1149,7 +1158,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1174,7 +1183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1224,7 +1233,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1283,13 +1292,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1298,13 +1316,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>